<commit_message>
Replace $ in conditions to #
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/testTemplate4.xlsx
+++ b/src/test/resources/templates/testTemplate4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\primary\mortgage\mortgage-pilot\reporting\src\test\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\primary\artezio\ART-BPMS-REPORTING-YARG\src\test\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="27870" windowHeight="12915"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="27870" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="testTemplate3" sheetId="1" r:id="rId1"/>
@@ -49,13 +49,13 @@
     <t>${extraItem.price}</t>
   </si>
   <si>
-    <t>${IF ${price} &gt; 20}Expensive${ELSE}Cheap${ENDIF}</t>
-  </si>
-  <si>
     <t>Expression result</t>
   </si>
   <si>
     <t>#{${price} * 3}</t>
+  </si>
+  <si>
+    <t>#{IF ${price} &gt; 20}Expensive#{ELSE}Cheap#{ENDIF}</t>
   </si>
 </sst>
 </file>
@@ -883,7 +883,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -920,10 +920,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>